<commit_message>
Fixed the LD1 naming of LD2 in BOM
</commit_message>
<xml_diff>
--- a/Diag586220_Harness/Diag586220_Cassette_Port/Rev.1/excel/Diag586220_Cassette_BOM_v1_0.xlsx
+++ b/Diag586220_Harness/Diag586220_Cassette_Port/Rev.1/excel/Diag586220_Cassette_BOM_v1_0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Projekte\_Eigene\C64-Projects\Diag586220_Harness\Diag586220_Cassette_Port\Rev.1\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9018E0-CE52-41DF-AD92-8EFB8454DEB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7EAC72-5125-4FFB-8CED-E98BC62C69B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="3552" windowWidth="21012" windowHeight="13728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3996" yWindow="2028" windowWidth="21012" windowHeight="13728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stückliste" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Pos.</t>
   </si>
@@ -164,19 +164,28 @@
   </si>
   <si>
     <t>2 layer, Cu 35µ, HASL, 30.0mm x 43.0mm, 1.6mm FR4</t>
+  </si>
+  <si>
+    <t>LD2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Futura Lt BT"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -642,49 +651,49 @@
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -692,10 +701,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -707,19 +716,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -728,17 +743,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -922,7 +934,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A3:F13" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A3:F13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A4:F37">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:F37">
     <sortCondition ref="E3:E37"/>
   </sortState>
   <tableColumns count="6">
@@ -1239,7 +1251,7 @@
   <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1452,8 +1464,8 @@
       <c r="D11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>11</v>
+      <c r="E11" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>38</v>

</xml_diff>